<commit_message>
updated main module upload report done
</commit_message>
<xml_diff>
--- a/WebContent/UploadedFiles/Report.xlsx
+++ b/WebContent/UploadedFiles/Report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>ID</t>
   </si>
@@ -34,10 +34,19 @@
     <t>Krishna Biswas</t>
   </si>
   <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>"28/10/21"</t>
+  </si>
+  <si>
     <t>2:35PM</t>
   </si>
   <si>
     <t>6:00PM</t>
+  </si>
+  <si>
+    <t>03:30:00AM</t>
   </si>
 </sst>
 </file>
@@ -75,7 +84,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,22 +389,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,16 +413,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5</v>
       </c>
@@ -420,13 +433,16 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0.14583333333333334</v>
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated main module attendance inert into database
</commit_message>
<xml_diff>
--- a/WebContent/UploadedFiles/Report.xlsx
+++ b/WebContent/UploadedFiles/Report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>ID</t>
   </si>
@@ -40,13 +40,28 @@
     <t>"28/10/21"</t>
   </si>
   <si>
-    <t>2:35PM</t>
-  </si>
-  <si>
-    <t>6:00PM</t>
-  </si>
-  <si>
-    <t>03:30:00AM</t>
+    <t>Avijit</t>
+  </si>
+  <si>
+    <t>"2:35PM"</t>
+  </si>
+  <si>
+    <t>"14:14PM"</t>
+  </si>
+  <si>
+    <t>"6:00PM"</t>
+  </si>
+  <si>
+    <t>"18:55PM"</t>
+  </si>
+  <si>
+    <t>"04:30"</t>
+  </si>
+  <si>
+    <t>"03:30"</t>
+  </si>
+  <si>
+    <t>"29/10/21"</t>
   </si>
 </sst>
 </file>
@@ -84,7 +99,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,17 +404,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
@@ -436,16 +451,37 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>